<commit_message>
Added validation to CSV - 1rst part
</commit_message>
<xml_diff>
--- a/storage/app/CSV/plantilla_usuarios.xlsx
+++ b/storage/app/CSV/plantilla_usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferzg\DinoCoffee\storage\app\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49162F5-459A-4432-A76A-3EB112408A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C44C529-A74E-476D-B3D6-C06713DBA4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Apellido Materno</t>
   </si>
@@ -47,115 +47,70 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Rol
+    <t>Fernando Augusto</t>
+  </si>
+  <si>
+    <t>Zavala</t>
+  </si>
+  <si>
+    <t>Gómez</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>+52 9993681035</t>
+  </si>
+  <si>
+    <t>ferzg2004@gmail.com</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Número Telefonico</t>
+  </si>
+  <si>
+    <t>Cumpleaños</t>
+  </si>
+  <si>
+    <t>Cedula profesional</t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>Maximo: 25 caracteres</t>
+  </si>
+  <si>
+    <t>Roles Permitidos:
 (ADM, DIR, COO, DOC, ALU)</t>
   </si>
   <si>
-    <t>Nombre/s</t>
-  </si>
-  <si>
-    <t>Matricula
-(25 caracteres max)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sexo
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>(F → Mujer | M → Hombre)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Número Telefonico
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>(+52 9993681035)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cumpleaños
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>(2004-06-05)</t>
-    </r>
-  </si>
-  <si>
-    <t>Fernando Augusto</t>
-  </si>
-  <si>
-    <t>Zavala</t>
-  </si>
-  <si>
-    <t>Gómez</t>
-  </si>
-  <si>
-    <t>ALU</t>
-  </si>
-  <si>
-    <t>+52 9993681035</t>
-  </si>
-  <si>
-    <t>ferzg2004@gmail.com</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cedula profesional
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>(Dejar vacio en caso de no tener)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>(Solo requerido para COO, DIR y DOC)</t>
-    </r>
+    <t>Solo:
+F → Mujer
+ M → Hombre</t>
+  </si>
+  <si>
+    <t>Formato:
++52 9993681035</t>
+  </si>
+  <si>
+    <t>Formato
+2004-06-05</t>
+  </si>
+  <si>
+    <t>* Dejar vacio en caso de no tener
+* Solo requerido para COO, DIR y DOC</t>
+  </si>
+  <si>
+    <t>Nombres</t>
   </si>
 </sst>
 </file>
@@ -165,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,24 +149,18 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="0"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Poppins"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
-      <color theme="0"/>
-      <name val="Poppins"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +179,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -244,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,7 +216,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -275,6 +230,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,110 +597,135 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="25.42578125" style="1"/>
-    <col min="5" max="5" width="50.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="3"/>
-    <col min="8" max="8" width="25.42578125" style="4"/>
-    <col min="9" max="9" width="35.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="25.42578125" style="1"/>
+    <col min="1" max="1" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="25.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="69.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>15221669</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="9">
-        <v>38143</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J3" s="5"/>
+      <c r="A3" s="7">
+        <v>15221669</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="9">
+        <v>38143</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J4" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E1048576">
+  <conditionalFormatting sqref="E3:E1048576">
     <cfRule type="expression" dxfId="4" priority="1">
-      <formula>NOT(OR(E2="ADM", E2="DIR", E2="COO", E2="DOC", E2="ALU", E2=""))</formula>
+      <formula>NOT(OR(E3="ADM", E3="DIR", E3="COO", E3="DOC", E3="ALU", E3=""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
+  <conditionalFormatting sqref="F3:F1048576">
     <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND(F2&lt;&gt;"F", F2&lt;&gt;"M", F2&lt;&gt;"")</formula>
+      <formula>AND(F3&lt;&gt;"F", F3&lt;&gt;"M", F3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="I2:I1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J2:J1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{8CC1EA68-19FC-45AD-87B1-AF27A7AE40E4}"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{8CC1EA68-19FC-45AD-87B1-AF27A7AE40E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>